<commit_message>
Local directory verandered naar TEMP-directory.
</commit_message>
<xml_diff>
--- a/Onderwijs/tm.xlsx
+++ b/Onderwijs/tm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Onderwijs\OnderwijsETTI\Onderwijs\Onderwijs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D1BF74-1D2D-4E9C-8FD3-EDC5FAC8FC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81423D8-ECA5-4770-8BB2-627F8C10C2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toetsmatrijs" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <definedName name="nmCompetenties">#REF!</definedName>
     <definedName name="nmNiveaus">#REF!</definedName>
     <definedName name="nmToetsvormen">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Toetsmatrijs!$A$1:$M$16</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -1480,6 +1481,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M560"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -2278,8 +2282,8 @@
       <formula1>nmToetsvormen</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>